<commit_message>
data overhaul, xlsx removed
</commit_message>
<xml_diff>
--- a/tests/testthat/data/day_14.xlsx
+++ b/tests/testthat/data/day_14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dyn4cast\tests\testthat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2147B930-3828-4957-9FDA-8CA226AEDC0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD38F39-06A0-4C24-8456-85134B7A2470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day_14" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,7 +520,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -872,14 +875,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="Q330" sqref="Q330"/>
+    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
+      <selection activeCell="E341" sqref="E341"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>

</xml_diff>